<commit_message>
cleared the test results flag for transmittals testcases.
</commit_message>
<xml_diff>
--- a/Fulcrum_Trunk/src/com/proj/suite/TRANSMITTALS Suite.xlsx
+++ b/Fulcrum_Trunk/src/com/proj/suite/TRANSMITTALS Suite.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FUL_PREPROD_DEC8\Fulcrum_PreProd_Trunk\src\com\proj\suite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WS_GIT_FUL\Fulcrum_Trunk\src\com\proj\suite\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>TCID</t>
   </si>
@@ -76,19 +76,12 @@
   </si>
   <si>
     <t>Verify Print option in Transmittals</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -517,16 +510,16 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E2" sqref="E2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="49.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="73.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.48828125" collapsed="true"/>
+    <col min="1" max="1" width="49.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="73.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -562,9 +555,7 @@
       <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
@@ -582,9 +573,7 @@
       <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
         <v>8</v>
       </c>
@@ -602,9 +591,7 @@
       <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
         <v>8</v>
       </c>

</xml_diff>